<commit_message>
SP commit before pull
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestCaseSettings.xlsx
+++ b/src/test/resources/TestData/TestCaseSettings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shiva\Downloads\calc\ZLatestJenkinsCode\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shiva\OneDrive\Desktop\GitCalcJenkins\Pulsora_Calculator\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D31DAC-5323-44A7-9E86-55BEFE8212FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1DAFEA6-1F92-4CB3-A8FF-3FA82C95D701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="105" yWindow="30" windowWidth="23895" windowHeight="12750" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UITestCases" sheetId="1" r:id="rId1"/>
@@ -940,22 +940,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMH34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C17" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29:E34"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="23.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="24" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="110.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="131.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="136.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" style="1" customWidth="1"/>
-    <col min="7" max="1022" width="8.6640625" style="1"/>
+    <col min="1" max="1" width="34.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="110.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="131.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="136.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" style="1" customWidth="1"/>
+    <col min="7" max="1022" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="37.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -990,7 +990,7 @@
       <c r="T1" s="3"/>
       <c r="U1" s="3"/>
     </row>
-    <row r="2" spans="1:21" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:21" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>7</v>
       </c>
@@ -1004,11 +1004,11 @@
         <v>24</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="F2" s="10"/>
     </row>
-    <row r="3" spans="1:21" ht="21" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:21" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>7</v>
       </c>
@@ -1022,11 +1022,11 @@
         <v>25</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="F3" s="10"/>
     </row>
-    <row r="4" spans="1:21" ht="21" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:21" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>7</v>
       </c>
@@ -1040,11 +1040,11 @@
         <v>26</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="F4" s="10"/>
     </row>
-    <row r="5" spans="1:21" ht="21" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:21" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>7</v>
       </c>
@@ -1058,11 +1058,11 @@
         <v>69</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="F5" s="10"/>
     </row>
-    <row r="6" spans="1:21" ht="21" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:21" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>7</v>
       </c>
@@ -1076,11 +1076,11 @@
         <v>28</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="F6" s="10"/>
     </row>
-    <row r="7" spans="1:21" ht="21" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:21" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>7</v>
       </c>
@@ -1094,11 +1094,11 @@
         <v>28</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="F7" s="10"/>
     </row>
-    <row r="8" spans="1:21" ht="21" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:21" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>7</v>
       </c>
@@ -1112,14 +1112,14 @@
         <v>31</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="F8" s="10"/>
       <c r="I8" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="21" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:21" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>7</v>
       </c>
@@ -1133,11 +1133,11 @@
         <v>33</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="F9" s="10"/>
     </row>
-    <row r="10" spans="1:21" ht="21" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:21" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
         <v>7</v>
       </c>
@@ -1151,11 +1151,11 @@
         <v>33</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="F10" s="10"/>
     </row>
-    <row r="11" spans="1:21" ht="21" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:21" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>7</v>
       </c>
@@ -1169,11 +1169,11 @@
         <v>82</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="F11" s="10"/>
     </row>
-    <row r="12" spans="1:21" ht="21" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:21" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>7</v>
       </c>
@@ -1191,7 +1191,7 @@
       </c>
       <c r="F12" s="10"/>
     </row>
-    <row r="13" spans="1:21" ht="21" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:21" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>7</v>
       </c>
@@ -1205,11 +1205,11 @@
         <v>78</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="F13" s="10"/>
     </row>
-    <row r="14" spans="1:21" ht="21" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:21" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>7</v>
       </c>
@@ -1223,11 +1223,11 @@
         <v>79</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="F14" s="10"/>
     </row>
-    <row r="15" spans="1:21" ht="21" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:21" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>7</v>
       </c>
@@ -1241,11 +1241,11 @@
         <v>35</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="F15" s="10"/>
     </row>
-    <row r="16" spans="1:21" ht="21" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:21" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
         <v>7</v>
       </c>
@@ -1259,11 +1259,11 @@
         <v>88</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="F16" s="10"/>
     </row>
-    <row r="17" spans="1:6" ht="21" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>7</v>
       </c>
@@ -1277,11 +1277,11 @@
         <v>85</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="F17" s="10"/>
     </row>
-    <row r="18" spans="1:6" ht="21" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
         <v>7</v>
       </c>
@@ -1295,11 +1295,11 @@
         <v>39</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="F18" s="10"/>
     </row>
-    <row r="19" spans="1:6" ht="21" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
         <v>7</v>
       </c>
@@ -1313,11 +1313,11 @@
         <v>93</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="F19" s="7"/>
     </row>
-    <row r="20" spans="1:6" ht="21" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
         <v>7</v>
       </c>
@@ -1331,11 +1331,11 @@
         <v>44</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="F20" s="10"/>
     </row>
-    <row r="21" spans="1:6" ht="21" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
         <v>7</v>
       </c>
@@ -1349,11 +1349,11 @@
         <v>42</v>
       </c>
       <c r="E21" s="21" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="F21" s="10"/>
     </row>
-    <row r="22" spans="1:6" ht="21" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
         <v>7</v>
       </c>
@@ -1367,11 +1367,11 @@
         <v>37</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="F22" s="10"/>
     </row>
-    <row r="23" spans="1:6" ht="21" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
         <v>7</v>
       </c>
@@ -1385,11 +1385,11 @@
         <v>9</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="F23" s="10"/>
     </row>
-    <row r="24" spans="1:6" ht="21" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A24" s="15" t="s">
         <v>7</v>
       </c>
@@ -1403,11 +1403,11 @@
         <v>9</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="F24" s="10"/>
     </row>
-    <row r="25" spans="1:6" ht="21" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A25" s="15" t="s">
         <v>7</v>
       </c>
@@ -1421,11 +1421,11 @@
         <v>49</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="F25" s="10"/>
     </row>
-    <row r="26" spans="1:6" ht="21" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="s">
         <v>7</v>
       </c>
@@ -1439,11 +1439,11 @@
         <v>50</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="F26" s="10"/>
     </row>
-    <row r="27" spans="1:6" ht="21" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
         <v>7</v>
       </c>
@@ -1457,11 +1457,11 @@
         <v>51</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="F27" s="10"/>
     </row>
-    <row r="28" spans="1:6" ht="21" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
         <v>7</v>
       </c>
@@ -1475,11 +1475,11 @@
         <v>10</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="F28" s="10"/>
     </row>
-    <row r="29" spans="1:6" ht="21" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
         <v>53</v>
       </c>
@@ -1497,7 +1497,7 @@
       </c>
       <c r="F29" s="10"/>
     </row>
-    <row r="30" spans="1:6" ht="21" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
         <v>53</v>
       </c>
@@ -1515,7 +1515,7 @@
       </c>
       <c r="F30" s="7"/>
     </row>
-    <row r="31" spans="1:6" ht="21" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A31" s="13" t="s">
         <v>53</v>
       </c>
@@ -1533,7 +1533,7 @@
       </c>
       <c r="F31" s="7"/>
     </row>
-    <row r="32" spans="1:6" ht="21" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A32" s="13" t="s">
         <v>53</v>
       </c>
@@ -1551,7 +1551,7 @@
       </c>
       <c r="F32" s="7"/>
     </row>
-    <row r="33" spans="1:6" ht="21" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A33" s="13" t="s">
         <v>53</v>
       </c>
@@ -1569,7 +1569,7 @@
       </c>
       <c r="F33" s="7"/>
     </row>
-    <row r="34" spans="1:6" ht="21" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A34" s="13" t="s">
         <v>53</v>
       </c>

</xml_diff>